<commit_message>
Updates to daily metrics code
</commit_message>
<xml_diff>
--- a/provider.xlsx
+++ b/provider.xlsx
@@ -19,16 +19,16 @@
     <t>practiceName</t>
   </si>
   <si>
-    <t>Rice-Contreras</t>
+    <t>Williams-Davis</t>
   </si>
   <si>
-    <t>Owens, Hall and Beasley</t>
+    <t>Gallagher-Perez</t>
   </si>
   <si>
-    <t>Chaney-Terry</t>
+    <t>Ross LLC</t>
   </si>
   <si>
-    <t>Weaver, Bruce and Moreno</t>
+    <t>Hull LLC</t>
   </si>
 </sst>
 </file>

</xml_diff>